<commit_message>
maj base de données
</commit_message>
<xml_diff>
--- a/Base de données.xlsx
+++ b/Base de données.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1a1131bd7c92ce12/Documents/INSA/2A/Informatique/Projet/project-INSAMaps/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="62" documentId="11_AD4D9D64A577C15A4A541880209E52BC5ADEDD8A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2639C857-22BD-4DA2-8F2E-3655C74493D8}"/>
+  <xr:revisionPtr revIDLastSave="82" documentId="11_AD4D9D64A577C15A4A541880209E52BC5ADEDD8A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2339FAC9-C95C-47B8-845F-C0940EDF611C}"/>
   <bookViews>
     <workbookView xWindow="2520" yWindow="2720" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -417,7 +417,7 @@
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -563,50 +563,110 @@
       <c r="A14" t="s">
         <v>14</v>
       </c>
+      <c r="B14">
+        <v>436</v>
+      </c>
+      <c r="C14">
+        <v>393</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>15</v>
       </c>
+      <c r="B15">
+        <v>581</v>
+      </c>
+      <c r="C15">
+        <v>398</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B16">
+        <v>697</v>
+      </c>
+      <c r="C16">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B17">
+        <v>711</v>
+      </c>
+      <c r="C17">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B18">
+        <v>776</v>
+      </c>
+      <c r="C18">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B19">
+        <v>787</v>
+      </c>
+      <c r="C19">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B20">
+        <v>846</v>
+      </c>
+      <c r="C20">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B21">
+        <v>849</v>
+      </c>
+      <c r="C21">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B22">
+        <v>415</v>
+      </c>
+      <c r="C22">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>23</v>
+      </c>
+      <c r="B23">
+        <v>270</v>
+      </c>
+      <c r="C23">
+        <v>477</v>
       </c>
     </row>
   </sheetData>

</xml_diff>